<commit_message>
normaliza tabela/cria tabela favorite e insere valores na mesma
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable-fav-songs.xlsx
+++ b/SpotifyClone-Non-NormalizedTable-fav-songs.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+  <si>
+    <t>ID</t>
+  </si>
   <si>
     <t>pessoa_usuaria</t>
   </si>
@@ -121,13 +124,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -434,86 +446,114 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="88.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="88.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="3">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="3">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="3">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>